<commit_message>
Added user ability to select types and colours.
</commit_message>
<xml_diff>
--- a/main/exampleSheet7.xlsx
+++ b/main/exampleSheet7.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="133">
   <si>
     <t>Evaluation</t>
   </si>
@@ -277,6 +277,12 @@
     <t>Expectation Code</t>
   </si>
   <si>
+    <t>Evaluation Type</t>
+  </si>
+  <si>
+    <t>Shortform and Colour</t>
+  </si>
+  <si>
     <t>A1</t>
   </si>
   <si>
@@ -289,6 +295,12 @@
     <t>A1.0</t>
   </si>
   <si>
+    <t>Overall Strand</t>
+  </si>
+  <si>
+    <t>O.X</t>
+  </si>
+  <si>
     <t>A2</t>
   </si>
   <si>
@@ -298,6 +310,9 @@
     <t>A2.0</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>A3</t>
   </si>
   <si>
@@ -307,6 +322,9 @@
     <t>A3.0</t>
   </si>
   <si>
+    <t>E</t>
+  </si>
+  <si>
     <t>A4</t>
   </si>
   <si>
@@ -316,20 +334,38 @@
     <t>A4.0</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>Listening to Understand: listen in order to understand and respond appropriately in a variety of situations for a variety of purposes</t>
+  </si>
+  <si>
+    <t>Assignment</t>
   </si>
   <si>
     <t>Speaking to Communicate: use speaking skills and strategies appropriately to communicate
 with different audiences for a variety of purpose</t>
   </si>
   <si>
+    <t>Project</t>
+  </si>
+  <si>
     <t>Reflecting on Skills and Strategies: reflect on and identify their strengths as listeners and speakers, areas for improvement, and the strategies they found most helpful in oral communication situations</t>
   </si>
   <si>
     <t>A1.3</t>
   </si>
   <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
     <t>Reading for Meaning: read and demonstrate an understanding of a variety of literary, informational, and graphic texts, using a range of strategies to construct meaning</t>
+  </si>
+  <si>
+    <t>Quiz</t>
   </si>
   <si>
     <t>Understanding Form and Style: recognize a variety of text forms, text features, and stylistic elements and demonstrate understanding of how they help communicate meaning</t>
@@ -381,7 +417,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="27">
+  <fonts count="36">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -436,6 +472,12 @@
     </font>
     <font>
       <b/>
+      <color rgb="FF34A853"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <color theme="8"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -447,6 +489,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color rgb="FFF1C232"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color rgb="FF34A853"/>
       <name val="Arial"/>
     </font>
@@ -457,11 +504,6 @@
     </font>
     <font>
       <color rgb="FFFF6D01"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color rgb="FFF1C232"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -499,6 +541,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <color rgb="FFC27BA0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="5"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -509,9 +556,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <color rgb="FF6AA84F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF9900FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FFC27BA0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FFFF00FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF4285F4"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -541,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -599,55 +677,55 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -658,7 +736,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -667,6 +748,33 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1983,290 +2091,290 @@
       <c r="B37" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="18" t="s">
         <v>59</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="18" t="s">
+      <c r="F37" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="18" t="s">
+      <c r="G37" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="H37" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J37" s="19" t="s">
+      <c r="J37" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="K37" s="19" t="s">
+      <c r="K37" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F38" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="24">
         <v>70.0</v>
       </c>
-      <c r="H38" s="23" t="s">
+      <c r="H38" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="J38" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="K38" s="24" t="s">
+      <c r="K38" s="21" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B39" s="22">
         <v>0.0</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="26" t="s">
         <v>70</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="F39" s="18" t="s">
+      <c r="F39" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="25">
         <v>15.0</v>
       </c>
-      <c r="H39" s="26"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
     </row>
     <row r="40">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" s="22">
         <v>25.0</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="26" t="s">
         <v>70</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="25">
         <v>15.0</v>
       </c>
-      <c r="H40" s="26"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
     </row>
     <row r="41">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="20">
+      <c r="B41" s="22">
         <v>35.0</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
+      <c r="C41" s="29"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
     </row>
     <row r="42">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" s="22">
         <v>44.0</v>
       </c>
-      <c r="C42" s="28"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
+      <c r="C42" s="29"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
     </row>
     <row r="43">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="22">
         <v>52.0</v>
       </c>
-      <c r="C43" s="21"/>
+      <c r="C43" s="23"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
       <c r="G43" s="14"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
     </row>
     <row r="44">
-      <c r="A44" s="20">
+      <c r="A44" s="22">
         <v>1.0</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="22">
         <v>55.0</v>
       </c>
-      <c r="C44" s="21"/>
+      <c r="C44" s="23"/>
       <c r="D44" s="13"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
     </row>
     <row r="45">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="22">
         <v>58.0</v>
       </c>
-      <c r="C45" s="11"/>
+      <c r="C45" s="23"/>
       <c r="D45" s="14"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
     </row>
     <row r="46">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="20">
+      <c r="B46" s="22">
         <v>62.0</v>
       </c>
-      <c r="C46" s="11"/>
+      <c r="C46" s="23"/>
       <c r="D46" s="14"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
     </row>
     <row r="47">
-      <c r="A47" s="20">
+      <c r="A47" s="22">
         <v>2.0</v>
       </c>
-      <c r="B47" s="20">
+      <c r="B47" s="22">
         <v>65.0</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="23"/>
       <c r="D47" s="14"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
     </row>
     <row r="48">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="20">
+      <c r="B48" s="22">
         <v>68.0</v>
       </c>
-      <c r="C48" s="28"/>
+      <c r="C48" s="29"/>
       <c r="D48" s="14"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
     </row>
     <row r="49">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B49" s="22">
         <v>72.0</v>
       </c>
-      <c r="C49" s="11"/>
+      <c r="C49" s="23"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
     </row>
     <row r="50">
-      <c r="A50" s="20">
+      <c r="A50" s="22">
         <v>3.0</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" s="22">
         <v>75.0</v>
       </c>
-      <c r="C50" s="11"/>
+      <c r="C50" s="23"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
     </row>
     <row r="51">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" s="22">
         <v>78.0</v>
       </c>
-      <c r="C51" s="11"/>
+      <c r="C51" s="23"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="27"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
     </row>
     <row r="52">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="29">
+      <c r="B52" s="30">
         <v>80.0</v>
       </c>
-      <c r="C52" s="30" t="s">
+      <c r="C52" s="31" t="s">
         <v>70</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
     </row>
     <row r="53">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="20">
+      <c r="B53" s="22">
         <v>86.0</v>
       </c>
-      <c r="C53" s="11"/>
+      <c r="C53" s="23"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
     </row>
     <row r="54">
-      <c r="A54" s="29">
+      <c r="A54" s="30">
         <v>4.0</v>
       </c>
-      <c r="B54" s="29">
+      <c r="B54" s="30">
         <v>91.0</v>
       </c>
-      <c r="C54" s="11"/>
+      <c r="C54" s="23"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
     </row>
     <row r="55">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B55" s="22">
         <v>94.0</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="31" t="s">
         <v>70</v>
       </c>
       <c r="D55" s="14"/>
@@ -2274,317 +2382,371 @@
       <c r="F55" s="14"/>
     </row>
     <row r="56">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="33"/>
+      <c r="C56" s="34"/>
     </row>
     <row r="57">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="C57" s="35" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="35"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="33"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="34"/>
     </row>
     <row r="59">
-      <c r="A59" s="35"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="33"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="34"/>
     </row>
     <row r="60">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="38" t="s">
+      <c r="B60" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="37" t="s">
+      <c r="C60" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="F60" s="39" t="s">
+      <c r="F60" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="G60" s="39" t="s">
+      <c r="G60" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="H60" s="39" t="s">
+      <c r="H60" s="40" t="s">
         <v>87</v>
       </c>
+      <c r="K60" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L60" s="42" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B61" s="41">
+      <c r="A61" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="44">
         <v>15.0</v>
       </c>
-      <c r="C61" s="41" t="s">
-        <v>89</v>
+      <c r="C61" s="44" t="s">
+        <v>91</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G61" s="39" t="s">
         <v>90</v>
       </c>
+      <c r="G61" s="40" t="s">
+        <v>92</v>
+      </c>
       <c r="H61" s="16" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+      <c r="K61" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="L61" s="45" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="44">
+        <v>35.0</v>
+      </c>
+      <c r="C62" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G62" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B62" s="41">
-        <v>35.0</v>
-      </c>
-      <c r="C62" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="F62" s="16" t="s">
+      <c r="H62" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K62" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="L62" s="46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="44">
+        <v>45.0</v>
+      </c>
+      <c r="C63" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="G62" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="H62" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B63" s="41">
-        <v>45.0</v>
-      </c>
-      <c r="C63" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="G63" s="39" t="s">
-        <v>90</v>
-      </c>
       <c r="H63" s="16" t="s">
-        <v>97</v>
+        <v>102</v>
+      </c>
+      <c r="K63" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="L63" s="47" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B64" s="41">
+      <c r="A64" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="44">
         <v>5.0</v>
       </c>
-      <c r="C64" s="41" t="s">
-        <v>99</v>
+      <c r="C64" s="44" t="s">
+        <v>105</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G64" s="39" t="s">
-        <v>90</v>
+        <v>104</v>
+      </c>
+      <c r="G64" s="40" t="s">
+        <v>92</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>100</v>
+        <v>106</v>
+      </c>
+      <c r="K64" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="L64" s="49" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="65">
       <c r="F65" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="H65" s="16" t="s">
         <v>16</v>
       </c>
+      <c r="K65" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="L65" s="50" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="66">
       <c r="F66" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="H66" s="16" t="s">
         <v>17</v>
       </c>
+      <c r="K66" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="L66" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="67">
       <c r="F67" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="H67" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="K67" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="L67" s="50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="F68" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G68" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H68" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="K68" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="L68" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="F69" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H69" s="51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="F70" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G70" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H70" s="51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="F71" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G71" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H71" s="51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="F72" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H72" s="51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="F73" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G73" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H73" s="51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="F74" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G74" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H74" s="51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="F75" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H75" s="51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="F76" s="51" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="F68" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="H68" s="42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="F69" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="H69" s="42" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="F70" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G70" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="H70" s="42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="F71" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="G71" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="H71" s="42" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="F72" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G72" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="H72" s="42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="F73" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H73" s="42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="F74" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G74" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="H74" s="42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="F75" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G75" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H75" s="42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="F76" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="G76" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="H76" s="42" t="s">
-        <v>115</v>
+        <v>126</v>
+      </c>
+      <c r="H76" s="51" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="77">
-      <c r="F77" s="42" t="s">
-        <v>98</v>
+      <c r="F77" s="51" t="s">
+        <v>104</v>
       </c>
       <c r="G77" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H77" s="42" t="s">
-        <v>117</v>
+        <v>128</v>
+      </c>
+      <c r="H77" s="51" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="78">
-      <c r="F78" s="42" t="s">
-        <v>98</v>
+      <c r="F78" s="51" t="s">
+        <v>104</v>
       </c>
       <c r="G78" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H78" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="H78" s="51" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="79">
-      <c r="F79" s="42" t="s">
-        <v>98</v>
+      <c r="F79" s="51" t="s">
+        <v>104</v>
       </c>
       <c r="G79" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="H79" s="42" t="s">
-        <v>120</v>
+        <v>131</v>
+      </c>
+      <c r="H79" s="51" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="83">
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="43"/>
+      <c r="B83" s="53"/>
+      <c r="C83" s="53"/>
+      <c r="D83" s="53"/>
+      <c r="E83" s="53"/>
     </row>
     <row r="84">
-      <c r="B84" s="44"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="44"/>
+      <c r="B84" s="54"/>
+      <c r="C84" s="55"/>
+      <c r="D84" s="54"/>
     </row>
     <row r="85">
-      <c r="B85" s="45"/>
-      <c r="C85" s="45"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="55"/>
     </row>
     <row r="86">
-      <c r="B86" s="44"/>
+      <c r="B86" s="54"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>